<commit_message>
optmized code with post program and put program
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
+++ b/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="Z0CkzYjVisrghyPSdlDYPM6sgKWEDgHFdp3cizLwRo4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="Ff6LpURyZ5aDEW2L7784IxFA3aUBpQm/ocr1pcjeQRg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Valid Credentials</t>
   </si>
   <si>
-    <t>Created</t>
-  </si>
-  <si>
     <t>ProgramName</t>
   </si>
   <si>
@@ -120,7 +117,7 @@
     <t>Java</t>
   </si>
   <si>
-    <t>Bad Request</t>
+    <t>cannot create program , since already exists</t>
   </si>
   <si>
     <t>Invalid Method</t>
@@ -135,6 +132,15 @@
     <t>Request method 'GET' is not supported</t>
   </si>
   <si>
+    <t>NoAuth</t>
+  </si>
+  <si>
+    <t>teamThreeProgram</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
     <t>Missing Values</t>
   </si>
   <si>
@@ -144,26 +150,107 @@
     <t>Invalid Request Body</t>
   </si>
   <si>
+    <t>kjhgui</t>
+  </si>
+  <si>
+    <t>programDescription must begin with letter and can only have letters, numbers, comma, hyphen, colon, period, underscore and space</t>
+  </si>
+  <si>
     <t>Mandatory</t>
   </si>
   <si>
-    <t>teamThreeProgram</t>
-  </si>
-  <si>
-    <t>OK</t>
+    <t>numpyningaprogsa</t>
   </si>
   <si>
     <t>Full Details</t>
   </si>
   <si>
-    <t>team-ThreeProgram</t>
+    <t>numpyninjaprogab</t>
+  </si>
+  <si>
+    <t>PutInvalidProgramId</t>
+  </si>
+  <si>
+    <t>putprogram/</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>ihfkd</t>
+  </si>
+  <si>
+    <t>PutInvalidRequestBodyByID</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
+  </si>
+  <si>
+    <t>PutWithoutRequestBodyByID</t>
+  </si>
+  <si>
+    <t>Required request body is missing</t>
+  </si>
+  <si>
+    <t>PutInvalidBaseURIByID</t>
+  </si>
+  <si>
+    <t>PutInvalidMethodByID</t>
+  </si>
+  <si>
+    <t>PutValidProgramIdWithNoAuth</t>
+  </si>
+  <si>
+    <t>teamThreePrograms</t>
+  </si>
+  <si>
+    <t>PutValidProgramId</t>
+  </si>
+  <si>
+    <t>System Applicationsss</t>
+  </si>
+  <si>
+    <t>PutInvalidProgramName</t>
+  </si>
+  <si>
+    <t>program/</t>
+  </si>
+  <si>
+    <t>no list with such program name</t>
+  </si>
+  <si>
+    <t>PutMissingMandatoryByName</t>
+  </si>
+  <si>
+    <t>PutInvalidValuesByName</t>
+  </si>
+  <si>
+    <t>PutInvalidProgramDescByName</t>
+  </si>
+  <si>
+    <t>programDescription must begin with letter and can only have letters</t>
+  </si>
+  <si>
+    <t>PutValidProgramNameWithNoAuth</t>
+  </si>
+  <si>
+    <t>InvalidToken</t>
+  </si>
+  <si>
+    <t>PutValidProgramName</t>
+  </si>
+  <si>
+    <t>PutStatusByProgramName</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -191,8 +278,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +300,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -226,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -251,6 +354,16 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,9 +794,7 @@
       <c r="G5" s="6">
         <v>200.0</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="H5" s="3"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -28525,14 +28636,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.29"/>
-    <col customWidth="1" min="2" max="2" width="21.29"/>
+    <col customWidth="1" min="1" max="1" width="35.29"/>
+    <col customWidth="1" min="2" max="2" width="24.29"/>
     <col customWidth="1" min="3" max="3" width="23.71"/>
     <col customWidth="1" min="4" max="4" width="18.86"/>
     <col customWidth="1" min="5" max="5" width="25.0"/>
     <col customWidth="1" min="6" max="7" width="25.43"/>
     <col customWidth="1" min="8" max="8" width="19.86"/>
-    <col customWidth="1" min="9" max="9" width="60.29"/>
+    <col customWidth="1" min="9" max="9" width="114.43"/>
     <col customWidth="1" min="10" max="27" width="8.71"/>
   </cols>
   <sheetData>
@@ -28550,13 +28661,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -28588,7 +28699,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>10</v>
@@ -28597,27 +28708,27 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="H2" s="8">
         <v>404.0</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>10</v>
@@ -28626,56 +28737,56 @@
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="8">
         <v>400.0</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="B4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="8">
         <v>405.0</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="B5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>10</v>
@@ -28683,26 +28794,26 @@
       <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="H5" s="8">
-        <v>400.0</v>
+        <v>401.0</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>10</v>
@@ -28710,28 +28821,26 @@
       <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8">
-        <v>1234.0</v>
-      </c>
+      <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="8">
         <v>400.0</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
@@ -28740,64 +28849,592 @@
         <v>11</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8">
+        <v>123445.0</v>
+      </c>
       <c r="G7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="9">
+        <v>201.0</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="9">
+        <v>201.0</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="8">
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="11">
+        <v>404.0</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="8">
+        <v>405.0</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="9">
         <v>200.0</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>43</v>
+      <c r="I16" s="12" t="s">
+        <v>39</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>44</v>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>31</v>
+      <c r="B17" s="8" t="s">
+        <v>64</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
+      <c r="D17" s="8" t="s">
+        <v>51</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>45</v>
+      <c r="E17" s="8" t="s">
+        <v>52</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>28</v>
+      <c r="H17" s="8">
+        <v>404.0</v>
       </c>
-      <c r="H8" s="8">
-        <v>201.0</v>
+      <c r="I17" s="8" t="s">
+        <v>65</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>21</v>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="8" t="s">
+        <v>66</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
+      <c r="B18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="8">
+        <v>123.0</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="8">
+        <v>123.0</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="9">
+        <v>200.0</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="9">
+        <v>200.0</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="10"/>
+    </row>
     <row r="25" ht="14.25" customHeight="1"/>
     <row r="26" ht="14.25" customHeight="1"/>
     <row r="27" ht="14.25" customHeight="1"/>
@@ -29774,6 +30411,9 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
get and delete program code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
+++ b/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="Ff6LpURyZ5aDEW2L7784IxFA3aUBpQm/ocr1pcjeQRg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="V7gfgs95oMe8R0X1XyBm5VQ3wOPA245uiiS1n805UL0="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="118">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -81,6 +81,21 @@
     <t>LmsHackathon@2024</t>
   </si>
   <si>
+    <t>Invalid Method</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Request method 'GET' is not supported</t>
+  </si>
+  <si>
+    <t>WithoutRequestBody</t>
+  </si>
+  <si>
+    <t>Required request body is missing</t>
+  </si>
+  <si>
     <t>Valid Credentials</t>
   </si>
   <si>
@@ -91,6 +106,9 @@
   </si>
   <si>
     <t>ProgramStatus</t>
+  </si>
+  <si>
+    <t>InvalidEndpoint</t>
   </si>
   <si>
     <t>saveprogra</t>
@@ -120,16 +138,7 @@
     <t>cannot create program , since already exists</t>
   </si>
   <si>
-    <t>Invalid Method</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
     <t>mnnjhj</t>
-  </si>
-  <si>
-    <t>Request method 'GET' is not supported</t>
   </si>
   <si>
     <t>NoAuth</t>
@@ -139,6 +148,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>PostWithoutRequestBody</t>
   </si>
   <si>
     <t>Missing Values</t>
@@ -168,7 +180,10 @@
     <t>numpyninjaprogab</t>
   </si>
   <si>
-    <t>PutInvalidProgramId</t>
+    <t>Update Program By ID</t>
+  </si>
+  <si>
+    <t>PutProgramByInvalidID</t>
   </si>
   <si>
     <t>putprogram/</t>
@@ -189,9 +204,6 @@
     <t>PutWithoutRequestBodyByID</t>
   </si>
   <si>
-    <t>Required request body is missing</t>
-  </si>
-  <si>
     <t>PutInvalidBaseURIByID</t>
   </si>
   <si>
@@ -210,7 +222,10 @@
     <t>System Applicationsss</t>
   </si>
   <si>
-    <t>PutInvalidProgramName</t>
+    <t>Update Program By Name</t>
+  </si>
+  <si>
+    <t>PutProgramByInvalidName</t>
   </si>
   <si>
     <t>program/</t>
@@ -237,6 +252,9 @@
     <t>InvalidToken</t>
   </si>
   <si>
+    <t>PutWithoutRequestBodyByName</t>
+  </si>
+  <si>
     <t>PutValidProgramName</t>
   </si>
   <si>
@@ -245,12 +263,123 @@
   <si>
     <t>Inactive</t>
   </si>
+  <si>
+    <t>Get Program By Id</t>
+  </si>
+  <si>
+    <t>GetProgramByInvalidID</t>
+  </si>
+  <si>
+    <t>programs/</t>
+  </si>
+  <si>
+    <t>GetProgramByIdWithInvalidMethod</t>
+  </si>
+  <si>
+    <t>Request method 'PUT' is not supported"</t>
+  </si>
+  <si>
+    <t>GetProgramByIdWithNoAuth</t>
+  </si>
+  <si>
+    <t>GetProgramByIdWithInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>programss/</t>
+  </si>
+  <si>
+    <t>GetProgramByIdWithInvalidBaseURI</t>
+  </si>
+  <si>
+    <t>GetProgramByvalidID</t>
+  </si>
+  <si>
+    <t>Get All Program With Users</t>
+  </si>
+  <si>
+    <t>GetAllProgramUsersWithInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>alProgramsWithUsers</t>
+  </si>
+  <si>
+    <t>GetAllProgramUsersWithInvalidMethod</t>
+  </si>
+  <si>
+    <t>allProgramsWithUsers</t>
+  </si>
+  <si>
+    <t>Request method 'PUT' is not supported</t>
+  </si>
+  <si>
+    <t>GetAllProgramUsersWithNoAuth</t>
+  </si>
+  <si>
+    <t>GetAllProgramUserWithInvalidBaseURI</t>
+  </si>
+  <si>
+    <t>GetAllProgramUsersValid</t>
+  </si>
+  <si>
+    <t>Get All Program With Admins</t>
+  </si>
+  <si>
+    <t>GetAllProgramWithInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>alPrograms</t>
+  </si>
+  <si>
+    <t>GetAllProgramWithInvalidMethod</t>
+  </si>
+  <si>
+    <t>allPrograms</t>
+  </si>
+  <si>
+    <t>GetAllProgramWithInvalidBaseURI</t>
+  </si>
+  <si>
+    <t>GetAllProgramWithNoAuth</t>
+  </si>
+  <si>
+    <t>GetAllProgramValid</t>
+  </si>
+  <si>
+    <t>Delete program By program Name</t>
+  </si>
+  <si>
+    <t>DeleteProgramByInvalidName</t>
+  </si>
+  <si>
+    <t>deletebyprogname/</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>no record found with programName</t>
+  </si>
+  <si>
+    <t>DeleteProgramByNameInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>DeleteProgramByNameInvalidMethod</t>
+  </si>
+  <si>
+    <t>DeleteProgramByNameInvalidBaseURI</t>
+  </si>
+  <si>
+    <t>DeleteProgramByNameNoAuth</t>
+  </si>
+  <si>
+    <t>DeleteProgramByValidName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -274,6 +403,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -286,10 +420,16 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,8 +444,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB6D7A8"/>
         <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
   </fills>
@@ -329,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -349,21 +507,72 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +804,8 @@
   <cols>
     <col customWidth="1" min="1" max="6" width="21.57"/>
     <col customWidth="1" min="7" max="7" width="10.43"/>
-    <col customWidth="1" min="8" max="26" width="21.57"/>
+    <col customWidth="1" min="8" max="8" width="34.86"/>
+    <col customWidth="1" min="9" max="26" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -773,28 +983,30 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="6">
-        <v>200.0</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>405.0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -815,14 +1027,26 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -843,32 +1067,46 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
+      <c r="A7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="10">
+        <v>200.0</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="2"/>
@@ -28617,6 +28855,62 @@
       <c r="X998" s="2"/>
       <c r="Y998" s="2"/>
       <c r="Z998" s="2"/>
+    </row>
+    <row r="999" ht="14.25" customHeight="1">
+      <c r="A999" s="2"/>
+      <c r="B999" s="2"/>
+      <c r="C999" s="2"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="2"/>
+      <c r="F999" s="2"/>
+      <c r="G999" s="2"/>
+      <c r="H999" s="2"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="2"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="2"/>
+      <c r="M999" s="2"/>
+      <c r="N999" s="2"/>
+      <c r="O999" s="2"/>
+      <c r="P999" s="2"/>
+      <c r="Q999" s="2"/>
+      <c r="R999" s="2"/>
+      <c r="S999" s="2"/>
+      <c r="T999" s="2"/>
+      <c r="U999" s="2"/>
+      <c r="V999" s="2"/>
+      <c r="W999" s="2"/>
+      <c r="X999" s="2"/>
+      <c r="Y999" s="2"/>
+      <c r="Z999" s="2"/>
+    </row>
+    <row r="1000" ht="14.25" customHeight="1">
+      <c r="A1000" s="2"/>
+      <c r="B1000" s="2"/>
+      <c r="C1000" s="2"/>
+      <c r="D1000" s="2"/>
+      <c r="E1000" s="2"/>
+      <c r="F1000" s="2"/>
+      <c r="G1000" s="2"/>
+      <c r="H1000" s="2"/>
+      <c r="I1000" s="2"/>
+      <c r="J1000" s="2"/>
+      <c r="K1000" s="2"/>
+      <c r="L1000" s="2"/>
+      <c r="M1000" s="2"/>
+      <c r="N1000" s="2"/>
+      <c r="O1000" s="2"/>
+      <c r="P1000" s="2"/>
+      <c r="Q1000" s="2"/>
+      <c r="R1000" s="2"/>
+      <c r="S1000" s="2"/>
+      <c r="T1000" s="2"/>
+      <c r="U1000" s="2"/>
+      <c r="V1000" s="2"/>
+      <c r="W1000" s="2"/>
+      <c r="X1000" s="2"/>
+      <c r="Y1000" s="2"/>
+      <c r="Z1000" s="2"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -28660,14 +28954,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>23</v>
+      <c r="E1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -28696,10 +28990,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>10</v>
@@ -28708,27 +29002,27 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H2" s="8">
         <v>404.0</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>10</v>
@@ -28737,56 +29031,56 @@
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H3" s="8">
         <v>400.0</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8">
         <v>405.0</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>10</v>
@@ -28795,25 +29089,25 @@
         <v>11</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H5" s="8">
         <v>401.0</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>10</v>
@@ -28822,25 +29116,21 @@
         <v>11</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="8">
         <v>400.0</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
@@ -28848,623 +29138,1407 @@
       <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="8">
-        <v>123445.0</v>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H7" s="8">
         <v>400.0</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="E8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="8">
+        <v>123445.0</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="13">
         <v>201.0</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="I9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="E10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="13">
         <v>201.0</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="10"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="8">
-        <v>404.0</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="I10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="8">
-        <v>400.0</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H12" s="8">
-        <v>400.0</v>
+        <v>404.0</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="11">
-        <v>404.0</v>
+        <v>42</v>
+      </c>
+      <c r="H13" s="8">
+        <v>400.0</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="8">
-        <v>405.0</v>
+        <v>400.0</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="8">
-        <v>401.0</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="H15" s="16">
+        <v>404.0</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="9">
-        <v>200.0</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
+      <c r="D16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="8">
+        <v>405.0</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="8">
-        <v>404.0</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="F18" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="8">
-        <v>400.0</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="G18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="13">
+        <v>200.0</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="8">
-        <v>123.0</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="8">
-        <v>400.0</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="8">
-        <v>123.0</v>
+        <v>57</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H20" s="8">
-        <v>400.0</v>
+        <v>404.0</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>38</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H21" s="8">
-        <v>401.0</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>39</v>
+        <v>400.0</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="E22" s="8">
+        <v>123.0</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="G22" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H22" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="8">
+        <v>123.0</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="8">
         <v>401.0</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="I24" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="9">
+      <c r="D25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8">
+        <v>400.0</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="13">
         <v>200.0</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="I27" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="14"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" s="9">
+      <c r="D28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="13">
         <v>200.0</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="10"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
+      <c r="I28" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="14"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="14"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="20">
+        <v>405.0</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="22">
+        <v>401.0</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="20">
+        <v>404.0</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="23">
+        <v>200.0</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14"/>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14"/>
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="8">
+        <v>405.0</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="A40" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25" customHeight="1">
+      <c r="A41" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="23">
+        <v>200.0</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+      <c r="Z41" s="14"/>
+      <c r="AA41" s="14"/>
+    </row>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="A42" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+    </row>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I43" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="8">
+        <v>405.0</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="8">
+        <v>404.0</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="A46" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="8">
+        <v>401.0</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="A47" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="23">
+        <v>200.0</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="14"/>
+      <c r="AA47" s="14"/>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+      <c r="Z48" s="14"/>
+      <c r="AA48" s="14"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="27">
+        <v>404.0</v>
+      </c>
+      <c r="I49" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="27">
+        <v>404.0</v>
+      </c>
+      <c r="I50" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="29">
+        <v>405.0</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" ht="14.25" customHeight="1">
+      <c r="A52" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="29">
+        <v>404.0</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="29">
+        <v>401.0</v>
+      </c>
+      <c r="I53" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="A54" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="30">
+        <v>200.0</v>
+      </c>
+      <c r="I54" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="14"/>
+      <c r="W54" s="14"/>
+      <c r="X54" s="14"/>
+      <c r="Y54" s="14"/>
+      <c r="Z54" s="14"/>
+      <c r="AA54" s="14"/>
+    </row>
     <row r="55" ht="14.25" customHeight="1"/>
     <row r="56" ht="14.25" customHeight="1"/>
     <row r="57" ht="14.25" customHeight="1"/>
@@ -30414,6 +31488,14 @@
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
+    <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
code changes with batch and program features
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
+++ b/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\Documents\2023_10_KanchanBasudkar\Team-3_APIWarriors_LMSHachathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C9EB91-0DCE-4490-BF4B-A6D1DDA6B909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A357C23-4448-47C2-A88A-0D845A3A6B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="94">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -180,12 +180,6 @@
     <t>batchId</t>
   </si>
   <si>
-    <t>batchDescription</t>
-  </si>
-  <si>
-    <t>batchNoOfClasses</t>
-  </si>
-  <si>
     <t>programName</t>
   </si>
   <si>
@@ -198,12 +192,6 @@
     <t>Existing batch Number</t>
   </si>
   <si>
-    <t>batch400</t>
-  </si>
-  <si>
-    <t>APIWarrwqs</t>
-  </si>
-  <si>
     <t>three</t>
   </si>
   <si>
@@ -213,13 +201,7 @@
     <t>MissingMandatoryField</t>
   </si>
   <si>
-    <t>APIWarrwqsw</t>
-  </si>
-  <si>
     <t>Missing additional fields</t>
-  </si>
-  <si>
-    <t>APIWarrwqswrsaax</t>
   </si>
   <si>
     <t>Invalid data</t>
@@ -231,16 +213,10 @@
     <t>Valid details</t>
   </si>
   <si>
-    <t>APIWarrwqswrsaaxq</t>
-  </si>
-  <si>
     <t>Invalid endpoint</t>
   </si>
   <si>
     <t>batch</t>
-  </si>
-  <si>
-    <t>APIWarrwqswrsaa</t>
   </si>
   <si>
     <t>Not Found</t>
@@ -289,6 +265,51 @@
   </si>
   <si>
     <t>programs/invalid/{programId}</t>
+  </si>
+  <si>
+    <t>ProgramId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid batchID and mandatory fields   </t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>APIWarriors001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid batchID and missing mandatory fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">update a batch with invalid data    </t>
+  </si>
+  <si>
+    <t>trywrongValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update a Batch with invalid enpoint </t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid batchID and deleted programID field  with other mandatory fields </t>
+  </si>
+  <si>
+    <t>update a Batch with a deleted batchID in the endpoint</t>
+  </si>
+  <si>
+    <t>valid batchID and mandatory fields in request body</t>
+  </si>
+  <si>
+    <t>invalid Program Id</t>
+  </si>
+  <si>
+    <t>invalid endpoint</t>
+  </si>
+  <si>
+    <t>deleted program id</t>
+  </si>
+  <si>
+    <t>valid Program Id</t>
   </si>
 </sst>
 </file>
@@ -416,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -442,6 +463,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28698,10 +28720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -28709,15 +28731,15 @@
     <col min="1" max="1" width="22.26953125" customWidth="1"/>
     <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="23.7265625" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="7" width="25.453125" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" customWidth="1"/>
-    <col min="9" max="9" width="60.26953125" customWidth="1"/>
-    <col min="10" max="27" width="8.7265625" customWidth="1"/>
+    <col min="4" max="5" width="18.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="8" width="25.453125" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" customWidth="1"/>
+    <col min="10" max="10" width="60.26953125" customWidth="1"/>
+    <col min="11" max="28" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14.25" customHeight="1">
+    <row r="1" spans="1:28" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -28731,21 +28753,23 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -28763,8 +28787,9 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
-    </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1">
+      <c r="AB1" s="2"/>
+    </row>
+    <row r="2" spans="1:28" ht="14.25" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -28777,23 +28802,24 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>404</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="14.5">
+    <row r="3" spans="1:28" ht="14.5">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -28806,23 +28832,24 @@
       <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>400</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="14.5">
+    <row r="4" spans="1:28" ht="14.5">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -28835,23 +28862,24 @@
       <c r="D4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>405</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="14.5">
+    <row r="5" spans="1:28" ht="14.5">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -28865,20 +28893,21 @@
         <v>11</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>400</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1">
+    <row r="6" spans="1:28" ht="14.25" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -28891,23 +28920,24 @@
       <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
         <v>1234</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>400</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1">
+    <row r="7" spans="1:28" ht="14.25" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -28920,21 +28950,22 @@
       <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>200</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1">
+    <row r="8" spans="1:28" ht="14.25" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -28947,25 +28978,26 @@
       <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="6">
         <v>201</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1">
+    <row r="9" spans="1:28" ht="14.25" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>31</v>
@@ -28977,56 +29009,57 @@
         <v>11</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="13">
+      <c r="I9" s="12"/>
+      <c r="J9" s="13">
         <v>401</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1">
+      <c r="K9" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="14.25" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="14.25" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E11" s="14">
         <v>16631</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1">
+    <row r="12" spans="1:28" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>10</v>
@@ -29037,19 +29070,19 @@
       <c r="E12" s="14">
         <v>16631</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>200</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1">
+      <c r="K12" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
@@ -29058,21 +29091,21 @@
         <v>35</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13">
+        <v>69</v>
+      </c>
+      <c r="J13">
         <v>404</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1">
+      <c r="K13" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>10</v>
@@ -29080,19 +29113,20 @@
       <c r="D14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I14">
+      <c r="E14" s="15"/>
+      <c r="J14">
         <v>404</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1">
+      <c r="K14" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="14.25" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>10</v>
@@ -29100,19 +29134,20 @@
       <c r="D15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I15">
+      <c r="E15" s="15"/>
+      <c r="J15">
         <v>401</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1">
+      <c r="K15" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>10</v>
@@ -29120,11 +29155,12 @@
       <c r="D16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I16">
+      <c r="E16" s="15"/>
+      <c r="J16">
         <v>404</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>71</v>
+      <c r="K16" s="12" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -30119,19 +30155,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA999"/>
+  <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="23" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14.25" customHeight="1">
+    <row r="1" spans="1:24" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -30157,23 +30193,17 @@
         <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -30184,16 +30214,13 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-    </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1">
+    </row>
+    <row r="2" spans="1:24" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -30201,11 +30228,11 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>56</v>
+      <c r="E2" t="s">
+        <v>82</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G2">
         <v>16331</v>
@@ -30213,31 +30240,22 @@
       <c r="H2">
         <v>10101</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2">
-        <v>99</v>
-      </c>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2">
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2">
         <v>400</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="14.25" customHeight="1">
+    <row r="3" spans="1:24" ht="14.25" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -30245,11 +30263,11 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>56</v>
+      <c r="E3" t="s">
+        <v>82</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3">
         <v>16331</v>
@@ -30257,31 +30275,22 @@
       <c r="H3">
         <v>10101</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3">
-        <v>99</v>
-      </c>
-      <c r="L3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3">
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3">
         <v>400</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="14.25" customHeight="1">
+    <row r="4" spans="1:24" ht="14.25" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -30289,11 +30298,11 @@
       <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>56</v>
+      <c r="E4" t="s">
+        <v>82</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4">
         <v>16331</v>
@@ -30301,29 +30310,22 @@
       <c r="H4">
         <v>10101</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4">
-        <v>99</v>
-      </c>
-      <c r="L4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4">
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4">
         <v>201</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -30331,11 +30333,11 @@
       <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>56</v>
+      <c r="E5" t="s">
+        <v>82</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5">
         <v>16331</v>
@@ -30344,30 +30346,21 @@
         <v>10101</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5">
+        <v>404</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K5">
-        <v>99</v>
-      </c>
-      <c r="L5" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5">
-        <v>404</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="B6" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>10</v>
@@ -30375,43 +30368,34 @@
       <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>56</v>
+      <c r="E6" t="s">
+        <v>82</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6">
         <v>16331</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6">
-        <v>12345</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6">
-        <v>99</v>
-      </c>
-      <c r="L6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6">
+        <v>400</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M6">
-        <v>400</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
@@ -30419,11 +30403,11 @@
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>56</v>
+      <c r="E7" t="s">
+        <v>82</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G7">
         <v>16335</v>
@@ -30431,31 +30415,22 @@
       <c r="H7">
         <v>10101</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7">
-        <v>99</v>
-      </c>
-      <c r="L7" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7">
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7">
         <v>400</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1">
+    <row r="8" spans="1:24" ht="14.25" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>10</v>
@@ -30463,11 +30438,11 @@
       <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>56</v>
+      <c r="E8" t="s">
+        <v>82</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G8">
         <v>16331</v>
@@ -30475,49 +30450,364 @@
       <c r="H8">
         <v>10101</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8">
-        <v>99</v>
-      </c>
-      <c r="L8" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8">
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8">
         <v>201</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9">
+        <v>16331</v>
+      </c>
+      <c r="H9">
+        <v>18000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9">
+        <v>404</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="H10">
+        <v>10101</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10">
+        <v>400</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11">
+        <v>16331</v>
+      </c>
+      <c r="H11">
+        <v>10101</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11">
+        <v>400</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12">
+        <v>16331</v>
+      </c>
+      <c r="H12">
+        <v>18000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12">
+        <v>404</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13">
+        <v>16407</v>
+      </c>
+      <c r="H13">
+        <v>10101</v>
+      </c>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13">
+        <v>400</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14">
+        <v>16331</v>
+      </c>
+      <c r="H14">
+        <v>8658</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14">
+        <v>200</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15">
+        <v>16331</v>
+      </c>
+      <c r="H15">
+        <v>10101</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15">
+        <v>200</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16">
+        <v>16335</v>
+      </c>
+      <c r="H16">
+        <v>10101</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16">
+        <v>404</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17">
+        <v>16331</v>
+      </c>
+      <c r="H17">
+        <v>10101</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17">
+        <v>404</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Neetu's code changes for Delete Batch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
+++ b/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\Documents\2023_10_KanchanBasudkar\Team-3_APIWarriors_LMSHachathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B5D41C-6349-40EA-9266-53924761B4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FC89A2-CA52-4EBE-9BC1-861737A8341F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="174">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -518,16 +518,56 @@
   <si>
     <t>GetBatchByProgramIdNoAuth</t>
   </si>
+  <si>
+    <t>DeletebatchvalidbatchId</t>
+  </si>
+  <si>
+    <t>batches/</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>DeletebatchInvalidbatchId</t>
+  </si>
+  <si>
+    <t>batches/12</t>
+  </si>
+  <si>
+    <t>not found</t>
+  </si>
+  <si>
+    <t>DeleteBatchInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>DeleteBatchInvalidMethod</t>
+  </si>
+  <si>
+    <t>Request method 'POST' is not supported</t>
+  </si>
+  <si>
+    <t>DeleteBatchInvalidNoAuth</t>
+  </si>
+  <si>
+    <t>Delete Batch by Batch Id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -588,6 +628,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -627,7 +685,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -661,75 +719,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31807,8 +31907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -31828,54 +31928,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
@@ -31895,264 +31995,264 @@
       <c r="AB2" s="11"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="37">
         <v>16331</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="37">
         <v>10101</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="37">
         <v>400</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="37">
         <v>16331</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="37">
         <v>10101</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="37">
         <v>400</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="37">
         <v>16331</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="37">
         <v>10101</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="37">
         <v>201</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="36" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="37">
         <v>16331</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="37">
         <v>10101</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="37">
         <v>404</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="37">
         <v>16331</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="37">
         <v>400</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="37">
         <v>16335</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="37">
         <v>10101</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="37">
         <v>400</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="37">
         <v>16331</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="37">
         <v>10101</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="37">
         <v>201</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="36" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="11"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -32172,259 +32272,260 @@
       <c r="AB10" s="11"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="37">
         <v>16331</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="37">
         <v>18000</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="37">
         <v>404</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="H12">
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37">
         <v>10101</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="37">
         <v>400</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="37">
         <v>16331</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="37">
         <v>10101</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="37">
         <v>400</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="37">
         <v>16331</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="37">
         <v>18000</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="37">
         <v>404</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="37">
         <v>16407</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="37">
         <v>10101</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="37">
         <v>400</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="37">
         <v>16331</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="37">
         <v>8658</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="37">
         <v>200</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="36" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="37">
         <v>16331</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="37">
         <v>10101</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="37">
         <v>200</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="36" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="11"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
@@ -32444,186 +32545,357 @@
       <c r="AB18" s="11"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="37">
         <v>16335</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="37">
         <v>10101</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="37">
         <v>404</v>
       </c>
-      <c r="K19" s="29" t="s">
+      <c r="K19" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
+      <c r="A20" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="37">
         <v>16335</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="37">
         <v>10101</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="37">
         <v>404</v>
       </c>
-      <c r="K20" s="29" t="s">
+      <c r="K20" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
+      <c r="A21" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="37">
         <v>16331</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="37">
         <v>10101</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="37">
         <v>404</v>
       </c>
-      <c r="K21" s="29" t="s">
+      <c r="K21" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="37">
         <v>16331</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="37">
         <v>10101</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="37">
         <v>404</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
+      <c r="A23" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="37">
         <v>16331</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="37">
         <v>10101</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="37">
         <v>200</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K23" s="36" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A24" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+    </row>
+    <row r="25" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A25" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37">
+        <v>10101</v>
+      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="42">
+        <v>200</v>
+      </c>
+      <c r="K25" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A26" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37">
+        <v>10101</v>
+      </c>
+      <c r="I26" s="37"/>
+      <c r="J26" s="42">
+        <v>404</v>
+      </c>
+      <c r="K26" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A27" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37">
+        <v>10101</v>
+      </c>
+      <c r="I27" s="37"/>
+      <c r="J27" s="42">
+        <v>404</v>
+      </c>
+      <c r="K27" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A28" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37">
+        <v>10101</v>
+      </c>
+      <c r="I28" s="37"/>
+      <c r="J28" s="42">
+        <v>405</v>
+      </c>
+      <c r="K28" s="44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A29" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37">
+        <v>10101</v>
+      </c>
+      <c r="I29" s="37"/>
+      <c r="J29" s="42">
+        <v>401</v>
+      </c>
+      <c r="K29" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="30" spans="1:28" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:28" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:28" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
code changes for get details by batch name and batch id
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
+++ b/src/test/resources/TestData/Team3-API Warriors Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\Documents\2023_10_KanchanBasudkar\Team-3_APIWarriors_LMSHachathon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FC89A2-CA52-4EBE-9BC1-861737A8341F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC0293C-4576-4769-A9D4-29AF0551C410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="185">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -551,16 +551,56 @@
   <si>
     <t>Delete Batch by Batch Id</t>
   </si>
+  <si>
+    <t>Get Batch Details by Batch Name</t>
+  </si>
+  <si>
+    <t>RetrieveBatchNoAuth</t>
+  </si>
+  <si>
+    <t>RetrieveBatchValidBatchName</t>
+  </si>
+  <si>
+    <t>RetrieveBatchInvalidBatchName</t>
+  </si>
+  <si>
+    <t>RetrieveBatchInvalidEndpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RetriveDeletedBatchName </t>
+  </si>
+  <si>
+    <t>RetrieveBatchByBatchIdNoAuth</t>
+  </si>
+  <si>
+    <t>RetrieveBatchValidBatchId</t>
+  </si>
+  <si>
+    <t>RetriveBatchDeletedBatchId</t>
+  </si>
+  <si>
+    <t>RetrieveBatchInvalidBatchId</t>
+  </si>
+  <si>
+    <t>Get Batch Details by Batch Id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -685,7 +725,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -734,101 +774,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -31905,10 +31960,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AB1004"/>
+  <dimension ref="A1:AB1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -32896,25 +32951,316 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A30" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+    </row>
+    <row r="31" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="42">
+        <v>200</v>
+      </c>
+      <c r="K31" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32" s="42">
+        <v>404</v>
+      </c>
+      <c r="K32" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="42">
+        <v>404</v>
+      </c>
+      <c r="K33" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J34" s="42">
+        <v>200</v>
+      </c>
+      <c r="K34" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J35" s="46">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A36" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+    </row>
+    <row r="37" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="37">
+        <v>10101</v>
+      </c>
+      <c r="J37" s="42">
+        <v>200</v>
+      </c>
+      <c r="K37" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>182</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H38" s="37">
+        <v>10101</v>
+      </c>
+      <c r="J38" s="42">
+        <v>200</v>
+      </c>
+      <c r="K38" s="40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="37">
+        <v>10101</v>
+      </c>
+      <c r="J39" s="42">
+        <v>404</v>
+      </c>
+      <c r="K39" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H40" s="37">
+        <v>10101</v>
+      </c>
+      <c r="J40" s="42">
+        <v>404</v>
+      </c>
+      <c r="K40" s="40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H41" s="37">
+        <v>10101</v>
+      </c>
+      <c r="J41" s="46">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:28" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -33869,8 +34215,6 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>